<commit_message>
CO cpu fix problem about "1"
</commit_message>
<xml_diff>
--- a/computer organization/hardwired/输出信号表.xlsx
+++ b/computer organization/hardwired/输出信号表.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git-repos\HomeWork\computer organization\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git-repos\HomeWork\computer organization\hardwired\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F785DDC2-142D-4152-8EF7-166CBCF16425}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D928572E-72CE-4EF1-BB97-8120DC53AD50}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16860" windowHeight="6945" activeTab="1" xr2:uid="{6005AAD0-0933-48B5-8F40-74FA52248108}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12443" windowHeight="4568" activeTab="1" xr2:uid="{6005AAD0-0933-48B5-8F40-74FA52248108}"/>
   </bookViews>
   <sheets>
     <sheet name="输出信号一览" sheetId="1" r:id="rId1"/>
@@ -292,18 +292,12 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>!ST</t>
-  </si>
-  <si>
     <t>SST</t>
   </si>
   <si>
     <t>W2&amp;!ST</t>
   </si>
   <si>
-    <t>ST</t>
-  </si>
-  <si>
     <t>W1&amp;!ST</t>
   </si>
   <si>
@@ -321,10 +315,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>!ST</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>右侧为扩展指令</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -350,6 +340,18 @@
   </si>
   <si>
     <t>S[0101]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>!ST&amp;W1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>!ST&amp;W1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ST&amp;W1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -851,10 +853,10 @@
   <dimension ref="A1:U39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R4" sqref="R4"/>
+      <selection pane="bottomRight" activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -895,7 +897,7 @@
         <v>39</v>
       </c>
       <c r="K1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L1" t="s">
         <v>40</v>
@@ -916,16 +918,16 @@
         <v>60</v>
       </c>
       <c r="R1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="S1" t="s">
+        <v>74</v>
+      </c>
+      <c r="T1" t="s">
         <v>77</v>
       </c>
-      <c r="T1" t="s">
-        <v>80</v>
-      </c>
       <c r="U1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.4">
@@ -933,7 +935,7 @@
         <v>10</v>
       </c>
       <c r="M2" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="P2" t="s">
         <v>63</v>
@@ -955,19 +957,19 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
+        <v>66</v>
+      </c>
+      <c r="M4" t="s">
+        <v>80</v>
+      </c>
+      <c r="N4" t="s">
         <v>67</v>
       </c>
-      <c r="M4" t="s">
-        <v>66</v>
-      </c>
-      <c r="N4" t="s">
-        <v>68</v>
-      </c>
       <c r="P4" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="Q4" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.4">
@@ -978,7 +980,7 @@
         <v>41</v>
       </c>
       <c r="M5" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="N5" t="s">
         <v>61</v>
@@ -1019,16 +1021,16 @@
         <v>41</v>
       </c>
       <c r="K6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="S6" t="s">
         <v>41</v>
       </c>
       <c r="T6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="U6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.4">
@@ -1051,10 +1053,10 @@
         <v>41</v>
       </c>
       <c r="T7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="U7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.4">
@@ -1088,16 +1090,16 @@
         <v>41</v>
       </c>
       <c r="K9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="S9" t="s">
         <v>41</v>
       </c>
       <c r="T9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="U9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.4">
@@ -1113,13 +1115,13 @@
         <v>0</v>
       </c>
       <c r="M11" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="N11" t="s">
         <v>61</v>
       </c>
       <c r="P11" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="Q11" t="s">
         <v>63</v>
@@ -1133,7 +1135,7 @@
         <v>47</v>
       </c>
       <c r="P12" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.4">
@@ -1144,7 +1146,7 @@
         <v>47</v>
       </c>
       <c r="Q13" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.4">
@@ -1158,10 +1160,10 @@
         <v>41</v>
       </c>
       <c r="P14" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="Q14" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.4">
@@ -1174,10 +1176,10 @@
         <v>13</v>
       </c>
       <c r="P16" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="Q16" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.4">
@@ -1199,7 +1201,7 @@
         <v>41</v>
       </c>
       <c r="M18" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.4">
@@ -1265,10 +1267,10 @@
         <v>41</v>
       </c>
       <c r="T24" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="U24" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.4">
@@ -1292,7 +1294,7 @@
         <v>41</v>
       </c>
       <c r="T27" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.4">
@@ -1322,7 +1324,7 @@
         <v>47</v>
       </c>
       <c r="K30" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.4">
@@ -1338,18 +1340,18 @@
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="S32" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="U33" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.4">
@@ -1357,7 +1359,7 @@
         <v>52</v>
       </c>
       <c r="N34" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.4">
@@ -1365,7 +1367,7 @@
         <v>53</v>
       </c>
       <c r="N35" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.4">
@@ -1373,7 +1375,7 @@
         <v>54</v>
       </c>
       <c r="N36" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.4">
@@ -1381,7 +1383,7 @@
         <v>55</v>
       </c>
       <c r="N37" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.4">

</xml_diff>